<commit_message>
add a new fold
</commit_message>
<xml_diff>
--- a/毕业设计/毕设资料整理.xlsx
+++ b/毕业设计/毕设资料整理.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28">
   <si>
     <t>系统管理</t>
   </si>
@@ -27,6 +27,9 @@
     <t>车辆管理</t>
   </si>
   <si>
+    <t>线路管理</t>
+  </si>
+  <si>
     <t>配送管理</t>
   </si>
   <si>
@@ -78,16 +81,16 @@
     <t xml:space="preserve">车辆信息 (ID,编号, 类别, 名称, 承重量, 价格, 车辆说明，车辆状态，创建时间，修改时间) </t>
   </si>
   <si>
-    <t xml:space="preserve">客户信息 (ID，编号, 姓名, 电话, 地址，备注，客户状态，创建时间，修改时间) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">管理员信息表 (ID，User_Id,User_code,用户名，姓名, 密码,性别, 用户类型，用户状态，创建时间，修改时间) </t>
+    <t xml:space="preserve">客户信息 (ID，编号, 姓名, 电话, 地址，备注，客户状态，创建时间，修改时间，签收状态) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">管理员信息表 (ID，User_Id,User_code,用户名，姓名, 密码,性别, 用户类型，用户状态，创建时间，修改时间，签收状态) </t>
   </si>
   <si>
     <t>订单信息（ID,订单编号，发货人, 发货人电话, 付款方式，货物描述,运费，重量， 发货地址, 收货人, 收货人电话, 收货地址, 说明，订单状态，创建时间，修改时间）</t>
   </si>
   <si>
-    <t>货物信息（ID,货物编号，货物描述，货物状态，货物重量，货物数量，创建时间，修改时间）</t>
+    <t>货物信息（ID,货物编号，货物描述，货物状态，货物重量，货物体积，货物数量，创建时间，修改时间）</t>
   </si>
   <si>
     <t>货架信息（ID，货架编号，货架类型，货物总数量，货物编号，入库时间，出库时间，备注，仓库状态，创建时间，修改时间）</t>
@@ -104,8 +107,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
@@ -155,6 +158,37 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -178,37 +212,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
@@ -232,6 +235,35 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -257,36 +289,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -307,24 +310,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -337,103 +352,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -446,48 +491,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -555,26 +558,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -598,6 +581,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -606,10 +609,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -618,97 +621,97 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -717,12 +720,12 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -732,19 +735,19 @@
     <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1115,10 +1118,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A19" sqref="$A19:$XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1127,14 +1130,14 @@
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="18.75" customWidth="1"/>
     <col min="4" max="4" width="18.5" customWidth="1"/>
-    <col min="5" max="5" width="16.875" customWidth="1"/>
-    <col min="6" max="6" width="16.75" customWidth="1"/>
-    <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="14.625" customWidth="1"/>
-    <col min="10" max="10" width="7.25" customWidth="1"/>
+    <col min="5" max="7" width="16.875" customWidth="1"/>
+    <col min="8" max="8" width="16.75" customWidth="1"/>
+    <col min="9" max="9" width="17" customWidth="1"/>
+    <col min="10" max="10" width="14.625" customWidth="1"/>
+    <col min="12" max="12" width="7.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="47" customHeight="1" spans="1:10">
+    <row r="1" ht="47" customHeight="1" spans="1:12">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1144,116 +1147,126 @@
       <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="F1"/>
       <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="5"/>
-    </row>
-    <row r="2" ht="14.25" spans="1:9">
+      <c r="K1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="5"/>
+    </row>
+    <row r="2" ht="14.25" spans="1:11">
       <c r="A2" s="3"/>
       <c r="C2" s="3"/>
       <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="I2" s="3"/>
-    </row>
-    <row r="3" ht="22" customHeight="1" spans="1:9">
+      <c r="K2" s="3"/>
+    </row>
+    <row r="3" ht="22" customHeight="1" spans="1:11">
       <c r="A3" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="I3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" ht="14.25" spans="1:5">
+      <c r="K3" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25" spans="1:7">
       <c r="A4" s="3"/>
       <c r="C4" s="3"/>
       <c r="E4" s="3"/>
-    </row>
-    <row r="5" ht="28" customHeight="1" spans="1:9">
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" ht="28" customHeight="1" spans="1:11">
       <c r="A5" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" t="s">
         <v>13</v>
       </c>
       <c r="I5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" ht="27" customHeight="1" spans="7:9">
-      <c r="G7" t="s">
+      <c r="K5" t="s">
         <v>15</v>
       </c>
+    </row>
+    <row r="7" ht="27" customHeight="1" spans="9:11">
       <c r="I7" t="s">
         <v>16</v>
       </c>
+      <c r="K7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="11" ht="25.5" spans="1:1">
       <c r="A11" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" s="1" customFormat="1" ht="26" customHeight="1" spans="1:1">
       <c r="A13" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" ht="28" customHeight="1" spans="1:1">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" ht="24" customHeight="1" spans="1:1">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" ht="21" customHeight="1" spans="1:1">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" ht="28" customHeight="1" spans="1:1">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" ht="29" customHeight="1" spans="1:1">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" ht="22" customHeight="1" spans="1:1">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" ht="25" customHeight="1" spans="1:1">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" ht="24" customHeight="1" spans="1:1">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>